<commit_message>
add some comments to clear up the code
</commit_message>
<xml_diff>
--- a/10_best_shops.xlsx
+++ b/10_best_shops.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>price</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>z_value</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -463,6 +468,9 @@
       <c r="D2" t="n">
         <v>2</v>
       </c>
+      <c r="E2" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -477,6 +485,9 @@
       <c r="D3" t="n">
         <v>4</v>
       </c>
+      <c r="E3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -491,6 +502,9 @@
       <c r="D4" t="n">
         <v>3</v>
       </c>
+      <c r="E4" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -505,6 +519,9 @@
       <c r="D5" t="n">
         <v>3</v>
       </c>
+      <c r="E5" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -519,6 +536,9 @@
       <c r="D6" t="n">
         <v>3</v>
       </c>
+      <c r="E6" t="n">
+        <v>87.05882352941177</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -533,6 +553,9 @@
       <c r="D7" t="n">
         <v>3</v>
       </c>
+      <c r="E7" t="n">
+        <v>83.75</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -547,6 +570,9 @@
       <c r="D8" t="n">
         <v>6</v>
       </c>
+      <c r="E8" t="n">
+        <v>71.25</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -561,6 +587,9 @@
       <c r="D9" t="n">
         <v>3</v>
       </c>
+      <c r="E9" t="n">
+        <v>71.25</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -575,6 +604,9 @@
       <c r="D10" t="n">
         <v>5</v>
       </c>
+      <c r="E10" t="n">
+        <v>70.45454545454545</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -588,6 +620,9 @@
       </c>
       <c r="D11" t="n">
         <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>68.33333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>